<commit_message>
US-11840 [FIX] Return from Unit export: Changed template
Signed-off-by: Dorian Kemps <dk@tempo-consulting.fr>
</commit_message>
<xml_diff>
--- a/bin/addons/msf_doc_import/report/return_from_unit_export.xlsx
+++ b/bin/addons/msf_doc_import/report/return_from_unit_export.xlsx
@@ -32,12 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
-    <t>Sending date:</t>
-  </si>
-  <si>
-    <t>Delivery date:</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -77,12 +71,6 @@
     <t>date and place:</t>
   </si>
   <si>
-    <t>Name and signature of the person in charge of delivery:</t>
-  </si>
-  <si>
-    <t>Executive name &amp; signature</t>
-  </si>
-  <si>
     <t>Date format</t>
   </si>
   <si>
@@ -90,6 +78,18 @@
   </si>
   <si>
     <t>Line date format</t>
+  </si>
+  <si>
+    <t>Creation date:</t>
+  </si>
+  <si>
+    <t>Expected Receipt date:</t>
+  </si>
+  <si>
+    <t>Sent by:</t>
+  </si>
+  <si>
+    <t>Received by:</t>
   </si>
 </sst>
 </file>
@@ -141,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -243,13 +243,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -312,6 +321,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -333,8 +345,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -733,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +783,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J2" s="18">
         <v>29250</v>
@@ -787,7 +799,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="1"/>
       <c r="I3" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J3" s="21">
         <v>29250</v>
@@ -803,7 +815,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="1"/>
       <c r="I4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J4" s="20">
         <v>0.01</v>
@@ -824,13 +836,13 @@
     <row r="6" spans="1:10" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="24"/>
+      <c r="C6" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="25"/>
       <c r="E6" s="7"/>
       <c r="F6" s="13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="1"/>
@@ -853,12 +865,12 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="1"/>
       <c r="F8" s="14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="1"/>
@@ -868,11 +880,11 @@
     <row r="9" spans="1:10" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -893,48 +905,48 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="12"/>
+      <c r="G11" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="30"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="D12" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16" t="s">
         <v>8</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>10</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="22">
         <v>1</v>
       </c>
       <c r="B13" s="2"/>
@@ -948,7 +960,7 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
+      <c r="A14" s="22">
         <v>2</v>
       </c>
       <c r="B14" s="2"/>
@@ -962,7 +974,7 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
+      <c r="A15" s="22">
         <v>3</v>
       </c>
       <c r="B15" s="2"/>
@@ -976,7 +988,7 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
+      <c r="A16" s="22">
         <v>4</v>
       </c>
       <c r="B16" s="2"/>
@@ -990,7 +1002,7 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
+      <c r="A17" s="22">
         <v>5</v>
       </c>
       <c r="B17" s="2"/>
@@ -1004,7 +1016,7 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="22">
         <v>6</v>
       </c>
       <c r="B18" s="2"/>
@@ -1018,7 +1030,7 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="A19" s="22">
         <v>7</v>
       </c>
       <c r="B19" s="2"/>
@@ -1032,7 +1044,7 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
+      <c r="A20" s="22">
         <v>8</v>
       </c>
       <c r="B20" s="2"/>
@@ -1046,7 +1058,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="22">
         <v>9</v>
       </c>
       <c r="B21" s="2"/>
@@ -1060,7 +1072,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
+      <c r="A22" s="22">
         <v>10</v>
       </c>
       <c r="B22" s="2"/>
@@ -1085,19 +1097,19 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="22"/>
+      <c r="B24" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="23"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="22"/>
+      <c r="G24" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="23"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
@@ -1125,17 +1137,17 @@
     </row>
     <row r="27" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="23"/>
+      <c r="B27" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="24"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="23"/>
+      <c r="G27" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="24"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
@@ -1200,7 +1212,7 @@
       <c r="J32" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="G24:H24"/>
@@ -1208,6 +1220,7 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>